<commit_message>
visualize neighborhoods that are being compared with the plotProportions function
</commit_message>
<xml_diff>
--- a/bugs/Exploring Z score.xlsx
+++ b/bugs/Exploring Z score.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27618"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27624"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="49" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF7DC48A-B56D-4428-BADF-8BA5C8EE3A6E}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C32861F6-1188-4583-AA94-0853AC120A27}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>y1</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Z</t>
+  </si>
+  <si>
+    <t>More cells, but same proportions.</t>
   </si>
 </sst>
 </file>
@@ -87,8 +90,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,15 +429,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -454,7 +460,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
@@ -481,7 +487,7 @@
         <v>-2.5955427380922007</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>1</v>
       </c>
@@ -508,7 +514,7 @@
         <v>-2.5361704997929655</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>18</v>
       </c>
@@ -536,7 +542,7 @@
         <v>-5.3033008588991075</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>18</v>
       </c>
@@ -564,7 +570,7 @@
         <v>-4.3211340143675807</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>30</v>
       </c>
@@ -591,7 +597,7 @@
         <v>-5.6493268286603211</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>180</v>
       </c>
@@ -619,7 +625,181 @@
         <v>-16.770509831248425</v>
       </c>
     </row>
+    <row r="8" spans="1:10">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <f>A8*2</f>
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ref="D8" si="4">A8/C8</f>
+        <v>0.1</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ref="E8" si="5">B8/C8</f>
+        <v>0.2</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ref="F8" si="6">(A8+B8)/(2*C8)</f>
+        <v>0.15</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ref="G8" si="7">(D8-E8) / ( SQRT( 2*F8*(1-F8)/C8 ) )</f>
+        <v>-1.9802950859533488</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9">
+        <v>100</v>
+      </c>
+      <c r="B9">
+        <v>200</v>
+      </c>
+      <c r="C9">
+        <v>1000</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ref="D9" si="8">A9/C9</f>
+        <v>0.1</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ref="E9" si="9">B9/C9</f>
+        <v>0.2</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9" si="10">(A9+B9)/(2*C9)</f>
+        <v>0.15</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ref="G9" si="11">(D9-E9) / ( SQRT( 2*F9*(1-F9)/C9 ) )</f>
+        <v>-6.2622429108514943</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>1000</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="D10" si="12">A10/C10</f>
+        <v>0.01</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ref="E10" si="13">B10/C10</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ref="F10" si="14">(A10+B10)/(2*C10)</f>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ref="G10" si="15">(D10-E10) / ( SQRT( 2*F10*(1-F10)/C10 ) )</f>
+        <v>1.2958630811567069</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11">
+        <v>60</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>1000</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11" si="16">A11/C11</f>
+        <v>0.06</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ref="E11" si="17">B11/C11</f>
+        <v>0.03</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ref="F11" si="18">(A11+B11)/(2*C11)</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ref="G11" si="19">(D11-E11) / ( SQRT( 2*F11*(1-F11)/C11 ) )</f>
+        <v>3.2359240084528675</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12">
+        <v>100</v>
+      </c>
+      <c r="B12">
+        <v>50</v>
+      </c>
+      <c r="C12">
+        <v>1000</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ref="D12:D13" si="20">A12/C12</f>
+        <v>0.1</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ref="E12:E13" si="21">B12/C12</f>
+        <v>0.05</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12:F13" si="22">(A12+B12)/(2*C12)</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ref="G12:G13" si="23">(D12-E12) / ( SQRT( 2*F12*(1-F12)/C12 ) )</f>
+        <v>4.2447635997800894</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13">
+        <v>100</v>
+      </c>
+      <c r="B13">
+        <v>95</v>
+      </c>
+      <c r="C13">
+        <v>1000</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="20"/>
+        <v>0.1</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="21"/>
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="22"/>
+        <v>9.7500000000000003E-2</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="23"/>
+        <v>0.37690256528391242</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H8:J9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>